<commit_message>
Tentando fazer a lógica de loop com planilhas
</commit_message>
<xml_diff>
--- a/DATA_BASES/teste1.xlsx
+++ b/DATA_BASES/teste1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lborali\Desktop\software projects\automation_app\DATA_BASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58987DC-1FC4-4702-8283-590B9533DAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A514D19-493E-4B19-9643-7E086FCC3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Cliente</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>rodolfo</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Thais</t>
+  </si>
+  <si>
+    <t>Bernadete</t>
   </si>
 </sst>
 </file>
@@ -354,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A11" sqref="A8:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -382,7 +391,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Label para número de repetições
</commit_message>
<xml_diff>
--- a/DATA_BASES/teste1.xlsx
+++ b/DATA_BASES/teste1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lborali\Desktop\software projects\automation_app\DATA_BASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A514D19-493E-4B19-9643-7E086FCC3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3168E4A0-334D-49EE-9742-3B63271EC416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A8:A11"/>
+      <selection activeCell="A16" sqref="A9:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -406,9 +406,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G19" t="s">
-        <v>5</v>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>